<commit_message>
added missing team, added tiebreak to calcualation
</commit_message>
<xml_diff>
--- a/raw/Результати СинЛУК - Весна.xlsx
+++ b/raw/Результати СинЛУК - Весна.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
   <si>
     <t>▲ Город</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Минус один</t>
+  </si>
+  <si>
+    <t>Цинічні бандери</t>
   </si>
 </sst>
 </file>
@@ -572,10 +575,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Аркуш1"/>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,7 +1121,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -1130,10 +1133,10 @@
         <v>23</v>
       </c>
       <c r="E24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24">
         <v>7</v>
@@ -1141,19 +1144,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F25">
         <v>9</v>
@@ -1164,59 +1167,59 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D26">
         <v>22</v>
       </c>
       <c r="E26">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F26">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G26">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C27">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D27">
         <v>22</v>
       </c>
       <c r="E27">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F27">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G27">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D28">
         <v>22</v>
@@ -1225,67 +1228,67 @@
         <v>7</v>
       </c>
       <c r="F28">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G28">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C29">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D29">
         <v>22</v>
       </c>
       <c r="E29">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F29">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G29">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C30">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D30">
         <v>22</v>
       </c>
       <c r="E30">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F30">
         <v>7</v>
       </c>
       <c r="G30">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C31">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D31">
         <v>22</v>
@@ -1294,53 +1297,53 @@
         <v>7</v>
       </c>
       <c r="F31">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G31">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C32">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D32">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E32">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G32">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D33">
         <v>21</v>
       </c>
       <c r="E33">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F33">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G33">
         <v>6</v>
@@ -1348,22 +1351,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E34">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F34">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G34">
         <v>6</v>
@@ -1371,59 +1374,59 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D35">
         <v>20</v>
       </c>
       <c r="E35">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35">
         <v>6</v>
       </c>
       <c r="G35">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E36">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F36">
         <v>6</v>
       </c>
       <c r="G36">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D37">
         <v>19</v>
@@ -1432,76 +1435,76 @@
         <v>7</v>
       </c>
       <c r="F37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G37">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>22</v>
       </c>
       <c r="C38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E38">
         <v>7</v>
       </c>
       <c r="F38">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G38">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D39">
         <v>18</v>
       </c>
       <c r="E39">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F39">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G39">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C40">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D40">
         <v>18</v>
       </c>
       <c r="E40">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G40">
         <v>4</v>
@@ -1509,68 +1512,68 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C41">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D41">
         <v>18</v>
       </c>
       <c r="E41">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F41">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G41">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C42">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D42">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E42">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F42">
         <v>5</v>
       </c>
       <c r="G42">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>36</v>
       </c>
       <c r="C43">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D43">
         <v>17</v>
       </c>
       <c r="E43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G43">
         <v>6</v>
@@ -1578,53 +1581,53 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C44">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D44">
         <v>17</v>
       </c>
       <c r="E44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F44">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G44">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C45">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D45">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+      <c r="G45">
         <v>4</v>
-      </c>
-      <c r="F45">
-        <v>7</v>
-      </c>
-      <c r="G45">
-        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>28</v>
@@ -1633,44 +1636,44 @@
         <v>45</v>
       </c>
       <c r="D46">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E46">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F46">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G46">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C47">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D47">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E47">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F47">
         <v>4</v>
       </c>
       <c r="G47">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>36</v>
@@ -1679,10 +1682,10 @@
         <v>47</v>
       </c>
       <c r="D48">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F48">
         <v>4</v>
@@ -1693,13 +1696,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
         <v>36</v>
       </c>
       <c r="C49">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D49">
         <v>13</v>
@@ -1716,36 +1719,36 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C50">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E50">
         <v>4</v>
       </c>
       <c r="F50">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G50">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
         <v>28</v>
       </c>
       <c r="C51">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D51">
         <v>12</v>
@@ -1754,78 +1757,101 @@
         <v>4</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G51">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
         <v>28</v>
       </c>
       <c r="C52">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D52">
         <v>12</v>
       </c>
       <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52">
         <v>2</v>
       </c>
-      <c r="F52">
-        <v>5</v>
-      </c>
       <c r="G52">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C53">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D53">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G53">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
         <v>22</v>
       </c>
       <c r="C54">
+        <v>53</v>
+      </c>
+      <c r="D54">
+        <v>7</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>52</v>
       </c>
-      <c r="D54">
-        <v>7</v>
-      </c>
-      <c r="E54">
+      <c r="B55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55">
+        <v>53</v>
+      </c>
+      <c r="D55">
+        <v>7</v>
+      </c>
+      <c r="E55">
         <v>2</v>
       </c>
-      <c r="F54">
+      <c r="F55">
         <v>3</v>
       </c>
-      <c r="G54">
+      <c r="G55">
         <v>2</v>
       </c>
     </row>

</xml_diff>